<commit_message>
Added code for Extent reports : updated with field names
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/login.xlsx
+++ b/src/main/resources/excelFiles/login.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Pass@2018-01-23 14:51:01.246</t>
+  </si>
+  <si>
+    <t>Pass@2018-01-24 13:59:34.347</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>